<commit_message>
todos testes feitos (?)
</commit_message>
<xml_diff>
--- a/casos_teste.xlsx
+++ b/casos_teste.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENAI\Desktop\calcularJurosComposto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\calcularJurosComposto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BEA36B2-42C9-4984-AD5C-63A63D2D453F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF380893-68CB-4787-802D-B865EB90FB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{A2F9BA4C-A36A-4258-A268-5DBF12A8D887}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A2F9BA4C-A36A-4258-A268-5DBF12A8D887}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="casos_teste" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>ARQUIVOS</t>
   </si>
@@ -57,15 +57,6 @@
     <t>calcular_juros_compostos</t>
   </si>
   <si>
-    <t>ValueError("Valor inválido")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enviando algo que não seja um número  </t>
-  </si>
-  <si>
-    <t>"alex te amo"</t>
-  </si>
-  <si>
     <t>3500, 40</t>
   </si>
   <si>
@@ -75,12 +66,6 @@
     <t>Enviando menos que 3 valores</t>
   </si>
   <si>
-    <t>Enviando apenas números 0</t>
-  </si>
-  <si>
-    <t>0, 0, 0</t>
-  </si>
-  <si>
     <t>Enviando o capital como número negativo</t>
   </si>
   <si>
@@ -100,6 +85,69 @@
   </si>
   <si>
     <t>1000, 40, -2</t>
+  </si>
+  <si>
+    <t>Enviando o juros como número decimal</t>
+  </si>
+  <si>
+    <t>1000, 15.5, 1</t>
+  </si>
+  <si>
+    <t>(155, 1155)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enviando algo que não seja um número no lugar do capital </t>
+  </si>
+  <si>
+    <t>ola, 40, 2</t>
+  </si>
+  <si>
+    <t>TypeError("O capital investido deve ser um número (int ou float).")</t>
+  </si>
+  <si>
+    <t>Enviando algo que não seja um número no lugar dos juros</t>
+  </si>
+  <si>
+    <t>1000, "ola", 2</t>
+  </si>
+  <si>
+    <t>TypeError("A taxa de juros deve ser um número (int ou float).")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enviando algo que não seja um número no lugar do tempo </t>
+  </si>
+  <si>
+    <t>1000, 40, "ola"</t>
+  </si>
+  <si>
+    <t>TypeError("O tempo deve ser um número (int ou float).")</t>
+  </si>
+  <si>
+    <t>Enviando o número 0 no lugar do capital</t>
+  </si>
+  <si>
+    <t>0, 40, 2</t>
+  </si>
+  <si>
+    <t>ValueError("O capital deve ser um número maior que 0")</t>
+  </si>
+  <si>
+    <t>Enviando o número 0 no lugar do juros</t>
+  </si>
+  <si>
+    <t>1000, 0, 2</t>
+  </si>
+  <si>
+    <t>ValueError("O juros deve ser um número maior que 0")</t>
+  </si>
+  <si>
+    <t>Enviando o número 0 no lugar do tempo</t>
+  </si>
+  <si>
+    <t>1000, 40, 0</t>
+  </si>
+  <si>
+    <t>ValueError("O tempo deve ser um número maior que 0")</t>
   </si>
 </sst>
 </file>
@@ -135,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,12 +210,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -200,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -218,12 +260,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -245,9 +281,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -285,7 +321,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -391,7 +427,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -533,7 +569,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,19 +577,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30890DC-60CA-4727-A5C3-CCB6E703E19D}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -591,20 +627,20 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -615,13 +651,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -632,13 +668,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -649,13 +685,13 @@
         <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -666,13 +702,13 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -683,28 +719,99 @@
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>